<commit_message>
completed the read excel file
</commit_message>
<xml_diff>
--- a/excel files/data.xlsx
+++ b/excel files/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christian.saldana\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christian.saldana\python-workspace\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722C9AEC-2988-4CF0-B846-F5DBBAEAB07E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AC4B7F-E6CC-4771-85E8-DD2906D9FE25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Client Name</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>christianesl@gmail.com; christianesl@yahoo.com</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Hello dear client</t>
@@ -348,10 +345,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -362,113 +359,105 @@
     <col min="4" max="4" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>